<commit_message>
Added code to account for edge cases in address
</commit_message>
<xml_diff>
--- a/TestFiles/MLSDataRawSmallTesting.xlsx
+++ b/TestFiles/MLSDataRawSmallTesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65364EE-B0C7-4B07-B328-1AB087AC9491}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDF3CA4-5469-4AF1-B77B-5593F3C6AAC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1584" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HatcoSampleMLSData" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="507">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -1535,6 +1535,9 @@
   </si>
   <si>
     <t>Liz Rigney</t>
+  </si>
+  <si>
+    <t>20190468b</t>
   </si>
   <si>
     <t>Sue Walker</t>
@@ -2385,7 +2388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -4376,10 +4379,13 @@
         <v>20190468</v>
       </c>
       <c r="K52" t="s">
-        <v>488</v>
+        <v>505</v>
       </c>
       <c r="L52" t="s">
         <v>492</v>
+      </c>
+      <c r="N52" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -4413,11 +4419,14 @@
       <c r="J53">
         <v>20190661</v>
       </c>
-      <c r="K53" t="s">
-        <v>488</v>
+      <c r="K53">
+        <v>20190661</v>
       </c>
       <c r="L53" t="s">
         <v>492</v>
+      </c>
+      <c r="N53" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -4451,11 +4460,14 @@
       <c r="J54">
         <v>20190864</v>
       </c>
-      <c r="K54" t="s">
-        <v>488</v>
+      <c r="K54">
+        <v>20190864</v>
       </c>
       <c r="L54" t="s">
         <v>492</v>
+      </c>
+      <c r="N54" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -4489,11 +4501,14 @@
       <c r="J55">
         <v>20191017</v>
       </c>
-      <c r="K55" t="s">
-        <v>488</v>
+      <c r="K55">
+        <v>20191017</v>
       </c>
       <c r="L55" t="s">
         <v>492</v>
+      </c>
+      <c r="N55" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -4527,11 +4542,14 @@
       <c r="J56">
         <v>20191129</v>
       </c>
-      <c r="K56" t="s">
-        <v>488</v>
+      <c r="K56">
+        <v>20191129</v>
       </c>
       <c r="L56" t="s">
         <v>492</v>
+      </c>
+      <c r="N56" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -4680,16 +4698,13 @@
         <v>20190085</v>
       </c>
       <c r="K60">
-        <v>20190139</v>
+        <v>20190470</v>
       </c>
       <c r="L60" t="s">
         <v>490</v>
       </c>
-      <c r="M60" t="b">
-        <v>1</v>
-      </c>
       <c r="N60" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -4761,11 +4776,14 @@
       <c r="J62">
         <v>20190085</v>
       </c>
-      <c r="K62" t="s">
-        <v>488</v>
+      <c r="K62">
+        <v>20190260</v>
       </c>
       <c r="L62" t="s">
         <v>490</v>
+      </c>
+      <c r="N62" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -4799,11 +4817,14 @@
       <c r="J63">
         <v>20190085</v>
       </c>
-      <c r="K63" t="s">
-        <v>488</v>
+      <c r="K63">
+        <v>20190470</v>
       </c>
       <c r="L63" t="s">
         <v>490</v>
+      </c>
+      <c r="N63" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -4837,11 +4858,14 @@
       <c r="J64">
         <v>20190085</v>
       </c>
-      <c r="K64" t="s">
-        <v>488</v>
+      <c r="K64">
+        <v>20190470</v>
       </c>
       <c r="L64" t="s">
         <v>490</v>
+      </c>
+      <c r="N64" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -5688,11 +5712,14 @@
       <c r="J86">
         <v>20191129</v>
       </c>
-      <c r="K86" t="s">
-        <v>488</v>
+      <c r="K86">
+        <v>20191028</v>
       </c>
       <c r="L86" t="s">
         <v>493</v>
+      </c>
+      <c r="N86" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -5840,11 +5867,17 @@
       <c r="J90">
         <v>20191129</v>
       </c>
-      <c r="K90" t="s">
-        <v>488</v>
+      <c r="K90">
+        <v>20191129</v>
       </c>
       <c r="L90" t="s">
         <v>495</v>
+      </c>
+      <c r="M90" t="b">
+        <v>1</v>
+      </c>
+      <c r="N90" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -6075,7 +6108,7 @@
         <v>491</v>
       </c>
       <c r="N96" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>